<commit_message>
5th Nov Evening Commit
</commit_message>
<xml_diff>
--- a/Feature Development/EmployeeData.xlsx
+++ b/Feature Development/EmployeeData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jatink\My_AI_Projects\LMS_v2\Feature Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085782EE-CE65-4E49-9C79-CCE4D5720F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B314992B-6C8B-4555-BA9D-761EE6C1827D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>Employee ID</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>Last Name</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -494,30 +503,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -528,37 +536,40 @@
         <v>44</v>
       </c>
       <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>42</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>34</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -568,38 +579,41 @@
       <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1234567890</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>43</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>21</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -609,38 +623,41 @@
       <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1234123456</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>27</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>43</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>20</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>12</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>21</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -650,38 +667,41 @@
       <c r="C4" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>9870987650</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>17</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>31</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>32</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>43</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>33</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>35</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>21</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -691,44 +711,47 @@
       <c r="C5" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1234567898</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>17</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>39</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>27</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>43</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>40</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>11</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>41</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{84DBC3EC-A004-43E7-84E3-DDE9C79A0C44}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{D5D56086-D458-464E-8129-2EDCF71A9B04}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{8D8A2DA2-8B0C-426F-BE7E-C37F1D9298C0}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{D398588B-3B61-4957-9746-B5FE960FB010}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{84DBC3EC-A004-43E7-84E3-DDE9C79A0C44}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{D5D56086-D458-464E-8129-2EDCF71A9B04}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{8D8A2DA2-8B0C-426F-BE7E-C37F1D9298C0}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{D398588B-3B61-4957-9746-B5FE960FB010}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>